<commit_message>
Saving last completed lesson
Student is supposed to start the next lesson as soon as he enters the
app. That is why the last completed lesson should be saved into his
account.
</commit_message>
<xml_diff>
--- a/scripts bd/Licoes english app - controle.xlsx
+++ b/scripts bd/Licoes english app - controle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="24">
   <si>
     <t>Done?</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Karina</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Thiago</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -180,6 +189,17 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -203,7 +223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,8 +239,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -246,18 +268,22 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -265,6 +291,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -272,9 +299,44 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -516,14 +578,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:F74" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="B4:F74"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Done?" dataDxfId="4"/>
-    <tableColumn id="2" name="Project 1" dataDxfId="3"/>
-    <tableColumn id="3" name="Due By" dataDxfId="2"/>
-    <tableColumn id="4" name="Notes" dataDxfId="1"/>
-    <tableColumn id="5" name="Tested?" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:H74" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B4:H74"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Done?" dataDxfId="6"/>
+    <tableColumn id="2" name="Project 1" dataDxfId="5"/>
+    <tableColumn id="3" name="Due By" dataDxfId="4"/>
+    <tableColumn id="4" name="Notes" dataDxfId="3"/>
+    <tableColumn id="5" name="Tested?" dataDxfId="2"/>
+    <tableColumn id="6" name="ID" dataDxfId="1"/>
+    <tableColumn id="7" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -764,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F74"/>
+  <dimension ref="B1:H74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -779,12 +843,12 @@
     <col min="5" max="5" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="55" customHeight="1">
+    <row r="1" spans="2:8" ht="55" customHeight="1">
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
@@ -796,16 +860,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="7" customFormat="1" ht="17" customHeight="1">
+    <row r="2" spans="2:8" s="7" customFormat="1" ht="17" customHeight="1">
       <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="15">
         <v>42328</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="4.5" customHeight="1"/>
-    <row r="4" spans="2:6" s="3" customFormat="1" ht="16.5" customHeight="1">
+    <row r="3" spans="2:8" ht="4.5" customHeight="1"/>
+    <row r="4" spans="2:8" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -821,924 +885,1212 @@
       <c r="F4" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="14">
         <v>42307</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="2:8" ht="16.5" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="14">
         <v>42307</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G6" s="13">
+        <v>2</v>
+      </c>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4">
         <v>3</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="14">
         <v>42307</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G7" s="13">
+        <v>3</v>
+      </c>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="2:8" ht="16.5" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="4"/>
       <c r="F8" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G8" s="13">
+        <v>4</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="16.5" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4">
         <v>5</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="4"/>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G9" s="13">
+        <v>5</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="16.5" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
         <v>6</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="4"/>
       <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G10" s="13">
+        <v>6</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="16.5" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="4"/>
       <c r="F11" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G11" s="13">
+        <v>7</v>
+      </c>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:8" ht="16.5" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4">
         <v>7</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="4"/>
       <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G12" s="13">
+        <v>8</v>
+      </c>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="16.5" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4">
         <v>8</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="4"/>
       <c r="F13" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="16.5" customHeight="1">
+      <c r="G13" s="13">
+        <v>9</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="16.5" customHeight="1">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4">
         <v>9</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="4"/>
       <c r="F14" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="G14" s="13">
+        <v>10</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4">
         <v>10</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="4"/>
       <c r="F15" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="G15" s="13">
+        <v>11</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4">
         <v>11</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="4"/>
       <c r="F16" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="G16" s="13">
+        <v>12</v>
+      </c>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4">
         <v>12</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="4"/>
       <c r="F17" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="G17" s="13">
+        <v>13</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="4"/>
       <c r="F18" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="G18" s="13">
+        <v>14</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="4">
         <v>13</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="4"/>
       <c r="F19" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="G19" s="13">
+        <v>15</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="4">
         <v>14</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="4"/>
       <c r="F20" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="G20" s="13">
+        <v>16</v>
+      </c>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4">
         <v>15</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="4"/>
       <c r="F21" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="G21" s="13">
+        <v>17</v>
+      </c>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8">
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4">
         <v>16</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="4"/>
       <c r="F22" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:6">
+      <c r="G22" s="13">
+        <v>18</v>
+      </c>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="2:8">
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="4">
         <v>17</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="4"/>
       <c r="F23" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="G23" s="13">
+        <v>19</v>
+      </c>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:8">
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="4">
         <v>18</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="4"/>
       <c r="F24" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="G24" s="13">
+        <v>20</v>
+      </c>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8">
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="13"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="4"/>
       <c r="F25" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
+      <c r="G25" s="13">
+        <v>21</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8">
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="4">
         <v>19</v>
       </c>
-      <c r="D26" s="13"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="4"/>
       <c r="F26" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
+      <c r="G26" s="13">
+        <v>22</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="2:8">
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="4">
         <v>20</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="4"/>
       <c r="F27" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="G27" s="13">
+        <v>23</v>
+      </c>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="2:8">
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="4">
         <v>21</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="4"/>
       <c r="F28" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="G28" s="13">
+        <v>24</v>
+      </c>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="2:8">
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="4">
         <v>22</v>
       </c>
-      <c r="D29" s="13"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="4"/>
       <c r="F29" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="2:6">
+      <c r="G29" s="13">
+        <v>25</v>
+      </c>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="2:8">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="4">
         <v>23</v>
       </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="4"/>
       <c r="F30" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="2:6">
+      <c r="G30" s="13">
+        <v>26</v>
+      </c>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="2:8">
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="4">
         <v>24</v>
       </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="4"/>
       <c r="F31" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="2:6">
+      <c r="G31" s="13">
+        <v>27</v>
+      </c>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:8">
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="13"/>
+      <c r="D32" s="14"/>
       <c r="E32" s="4"/>
       <c r="F32" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="G32" s="13">
+        <v>28</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="2:8">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="4">
         <v>25</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="4"/>
       <c r="F33" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="2:6">
+      <c r="G33" s="13">
+        <v>29</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="2:8">
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="4">
         <v>26</v>
       </c>
-      <c r="D34" s="13"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="4"/>
       <c r="F34" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="2:6">
+      <c r="G34" s="13">
+        <v>30</v>
+      </c>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="2:8">
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="4">
         <v>27</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="4"/>
       <c r="F35" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="2:6">
+      <c r="G35" s="13">
+        <v>31</v>
+      </c>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="2:8">
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="4">
         <v>28</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="4"/>
       <c r="F36" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="2:6">
+      <c r="G36" s="13">
+        <v>32</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="2:8">
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="4">
         <v>29</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="4"/>
       <c r="F37" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="2:6">
+      <c r="G37" s="13">
+        <v>33</v>
+      </c>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="2:8">
       <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="4">
         <v>30</v>
       </c>
-      <c r="D38" s="13"/>
+      <c r="D38" s="14"/>
       <c r="E38" s="4"/>
       <c r="F38" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="2:6">
+      <c r="G38" s="13">
+        <v>34</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="2:8">
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="13"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="4"/>
       <c r="F39" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="2:6">
+      <c r="G39" s="13">
+        <v>35</v>
+      </c>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="2:8">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="4">
         <v>31</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="4"/>
       <c r="F40" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="2:6">
+      <c r="G40" s="13">
+        <v>36</v>
+      </c>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="2:8">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="4">
         <v>32</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="4"/>
       <c r="F41" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
+      <c r="G41" s="13">
+        <v>37</v>
+      </c>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="2:8">
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="4">
         <v>33</v>
       </c>
-      <c r="D42" s="13"/>
+      <c r="D42" s="14"/>
       <c r="E42" s="4"/>
       <c r="F42" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:6">
+      <c r="G42" s="13">
+        <v>38</v>
+      </c>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="2:8">
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="4">
         <v>34</v>
       </c>
-      <c r="D43" s="13"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="4"/>
       <c r="F43" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="2:6">
+      <c r="G43" s="13">
+        <v>39</v>
+      </c>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="2:8">
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="4">
         <v>35</v>
       </c>
-      <c r="D44" s="13"/>
+      <c r="D44" s="14"/>
       <c r="E44" s="4"/>
       <c r="F44" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="2:6">
+      <c r="G44" s="13">
+        <v>40</v>
+      </c>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="2:8">
       <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="4">
         <v>36</v>
       </c>
-      <c r="D45" s="13"/>
+      <c r="D45" s="14"/>
       <c r="E45" s="4"/>
       <c r="F45" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="2:6">
+      <c r="G45" s="13">
+        <v>41</v>
+      </c>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="2:8">
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="13"/>
+      <c r="D46" s="14"/>
       <c r="E46" s="4"/>
       <c r="F46" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="2:6">
+      <c r="G46" s="13">
+        <v>42</v>
+      </c>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="2:8">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="4">
         <v>37</v>
       </c>
-      <c r="D47" s="13"/>
+      <c r="D47" s="14"/>
       <c r="E47" s="4"/>
       <c r="F47" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="2:6">
+      <c r="G47" s="13">
+        <v>43</v>
+      </c>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="2:8">
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="4">
         <v>38</v>
       </c>
-      <c r="D48" s="13"/>
+      <c r="D48" s="14"/>
       <c r="E48" s="4"/>
       <c r="F48" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="2:6">
+      <c r="G48" s="13">
+        <v>44</v>
+      </c>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="2:8">
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="4">
         <v>39</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="4"/>
       <c r="F49" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="2:6">
+      <c r="G49" s="13">
+        <v>45</v>
+      </c>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="2:8">
       <c r="B50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="4">
         <v>40</v>
       </c>
-      <c r="D50" s="13"/>
+      <c r="D50" s="14"/>
       <c r="E50" s="4"/>
       <c r="F50" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="2:6">
+      <c r="G50" s="13">
+        <v>46</v>
+      </c>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="2:8">
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="4">
         <v>41</v>
       </c>
-      <c r="D51" s="13"/>
+      <c r="D51" s="14"/>
       <c r="E51" s="4"/>
       <c r="F51" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="2:6">
+      <c r="G51" s="13">
+        <v>47</v>
+      </c>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="2:8">
       <c r="B52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="4">
         <v>42</v>
       </c>
-      <c r="D52" s="13"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="4"/>
       <c r="F52" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="2:6">
+      <c r="G52" s="13">
+        <v>48</v>
+      </c>
+      <c r="H52" s="13"/>
+    </row>
+    <row r="53" spans="2:8">
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="13"/>
+      <c r="D53" s="14"/>
       <c r="E53" s="4"/>
       <c r="F53" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="2:6">
+      <c r="G53" s="13">
+        <v>49</v>
+      </c>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="2:8">
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="4">
         <v>43</v>
       </c>
-      <c r="D54" s="13"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="4"/>
       <c r="F54" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="2:6">
+      <c r="G54" s="13">
+        <v>50</v>
+      </c>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="2:8">
       <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="4">
         <v>44</v>
       </c>
-      <c r="D55" s="13"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="4"/>
       <c r="F55" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="2:6">
+      <c r="G55" s="13">
+        <v>51</v>
+      </c>
+      <c r="H55" s="13"/>
+    </row>
+    <row r="56" spans="2:8">
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="4">
         <v>45</v>
       </c>
-      <c r="D56" s="13"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="4"/>
       <c r="F56" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="2:6">
+      <c r="G56" s="13">
+        <v>52</v>
+      </c>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="2:8">
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="4">
         <v>46</v>
       </c>
-      <c r="D57" s="13"/>
+      <c r="D57" s="14"/>
       <c r="E57" s="4"/>
       <c r="F57" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="2:6">
+      <c r="G57" s="13">
+        <v>53</v>
+      </c>
+      <c r="H57" s="13"/>
+    </row>
+    <row r="58" spans="2:8">
       <c r="B58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="4">
         <v>47</v>
       </c>
-      <c r="D58" s="13"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="4"/>
       <c r="F58" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="2:6">
+      <c r="G58" s="13">
+        <v>54</v>
+      </c>
+      <c r="H58" s="13"/>
+    </row>
+    <row r="59" spans="2:8">
       <c r="B59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="4">
         <v>48</v>
       </c>
-      <c r="D59" s="13"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="4"/>
       <c r="F59" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="2:6">
+      <c r="G59" s="13">
+        <v>55</v>
+      </c>
+      <c r="H59" s="13"/>
+    </row>
+    <row r="60" spans="2:8">
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="13"/>
+      <c r="D60" s="14"/>
       <c r="E60" s="4"/>
       <c r="F60" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="2:6">
+      <c r="G60" s="13">
+        <v>56</v>
+      </c>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="2:8">
       <c r="B61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="4">
         <v>49</v>
       </c>
-      <c r="D61" s="13"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="4"/>
       <c r="F61" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="2:6">
+      <c r="G61" s="13">
+        <v>57</v>
+      </c>
+      <c r="H61" s="13"/>
+    </row>
+    <row r="62" spans="2:8">
       <c r="B62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="4">
         <v>50</v>
       </c>
-      <c r="D62" s="13"/>
+      <c r="D62" s="14"/>
       <c r="E62" s="4"/>
       <c r="F62" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="2:6">
+      <c r="G62" s="13">
+        <v>58</v>
+      </c>
+      <c r="H62" s="13"/>
+    </row>
+    <row r="63" spans="2:8">
       <c r="B63" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" s="4">
         <v>51</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D63" s="14">
         <v>42308</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="2:6">
+      <c r="G63" s="13">
+        <v>59</v>
+      </c>
+      <c r="H63" s="13"/>
+    </row>
+    <row r="64" spans="2:8">
       <c r="B64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="4">
         <v>52</v>
       </c>
-      <c r="D64" s="13"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="4"/>
       <c r="F64" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="2:6">
+      <c r="G64" s="13">
+        <v>60</v>
+      </c>
+      <c r="H64" s="13"/>
+    </row>
+    <row r="65" spans="2:8">
       <c r="B65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="4">
         <v>53</v>
       </c>
-      <c r="D65" s="13"/>
+      <c r="D65" s="14"/>
       <c r="E65" s="4"/>
       <c r="F65" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="2:6">
+      <c r="G65" s="13">
+        <v>61</v>
+      </c>
+      <c r="H65" s="13"/>
+    </row>
+    <row r="66" spans="2:8">
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="4">
         <v>54</v>
       </c>
-      <c r="D66" s="13"/>
+      <c r="D66" s="14"/>
       <c r="E66" s="4"/>
       <c r="F66" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="2:6">
+      <c r="G66" s="13">
+        <v>62</v>
+      </c>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="2:8">
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="13"/>
+      <c r="D67" s="14"/>
       <c r="E67" s="4"/>
       <c r="F67" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="2:6">
+      <c r="G67" s="13">
+        <v>63</v>
+      </c>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="2:8">
       <c r="B68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="4">
         <v>55</v>
       </c>
-      <c r="D68" s="13"/>
+      <c r="D68" s="14"/>
       <c r="E68" s="4"/>
       <c r="F68" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="2:6">
+      <c r="G68" s="13">
+        <v>64</v>
+      </c>
+      <c r="H68" s="13"/>
+    </row>
+    <row r="69" spans="2:8">
       <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="4">
         <v>56</v>
       </c>
-      <c r="D69" s="13"/>
+      <c r="D69" s="14"/>
       <c r="E69" s="4"/>
       <c r="F69" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="2:6">
+      <c r="G69" s="13">
+        <v>65</v>
+      </c>
+      <c r="H69" s="13"/>
+    </row>
+    <row r="70" spans="2:8">
       <c r="B70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="4">
         <v>57</v>
       </c>
-      <c r="D70" s="13"/>
+      <c r="D70" s="14"/>
       <c r="E70" s="4"/>
       <c r="F70" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="2:6">
+      <c r="G70" s="13">
+        <v>66</v>
+      </c>
+      <c r="H70" s="13"/>
+    </row>
+    <row r="71" spans="2:8">
       <c r="B71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C71" s="4">
         <v>58</v>
       </c>
-      <c r="D71" s="13"/>
+      <c r="D71" s="14"/>
       <c r="E71" s="4"/>
       <c r="F71" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="2:6">
+      <c r="G71" s="13">
+        <v>67</v>
+      </c>
+      <c r="H71" s="13"/>
+    </row>
+    <row r="72" spans="2:8">
       <c r="B72" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="4">
         <v>59</v>
       </c>
-      <c r="D72" s="13"/>
+      <c r="D72" s="14"/>
       <c r="E72" s="4"/>
       <c r="F72" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="2:6">
+      <c r="G72" s="13">
+        <v>68</v>
+      </c>
+      <c r="H72" s="13"/>
+    </row>
+    <row r="73" spans="2:8">
       <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C73" s="4">
         <v>60</v>
       </c>
-      <c r="D73" s="13"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="4"/>
       <c r="F73" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="2:6">
+      <c r="G73" s="13">
+        <v>69</v>
+      </c>
+      <c r="H73" s="13"/>
+    </row>
+    <row r="74" spans="2:8">
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="13"/>
+      <c r="D74" s="14"/>
       <c r="E74" s="4"/>
       <c r="F74" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="G74" s="13">
+        <v>70</v>
+      </c>
+      <c r="H74" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1754,7 +2106,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B74 F5:F74">
       <formula1>"Yes, No"</formula1>
     </dataValidation>

</xml_diff>